<commit_message>
new file for data selection
</commit_message>
<xml_diff>
--- a/PlayerPerformances.xlsx
+++ b/PlayerPerformances.xlsx
@@ -19118,7 +19118,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E334" t="n">
@@ -19174,7 +19174,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E335" t="n">
@@ -19230,7 +19230,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E336" t="n">
@@ -19454,7 +19454,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E340" t="n">
@@ -19510,7 +19510,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E341" t="n">
@@ -19566,7 +19566,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E342" t="n">
@@ -19622,7 +19622,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E343" t="n">
@@ -20742,7 +20742,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>BERLIN RECYCLING Volleys</t>
+          <t>Helios GRIZZLYS Giesen</t>
         </is>
       </c>
       <c r="E363" t="n">

</xml_diff>